<commit_message>
Stage.xlsx 의 MonsterTable 에 attackSpeed|Float 컬럼 추가 Actor.xlsx 의 ActorTable 에 attackSpeed|Float 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989EA6EB-C173-4766-B0C5-70E536786F89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A03DE3-6462-4A61-BFBF-EAE20A6E89A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
   <sheets>
     <sheet name="ActorTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Actor002</t>
   </si>
@@ -106,6 +106,10 @@
   </si>
   <si>
     <t>def|Float</t>
+  </si>
+  <si>
+    <t>attackSpeed|Float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -472,18 +476,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAEF85E-644F-4CA8-8208-63C893B0C10A}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="19.375" customWidth="1"/>
     <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="16.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -496,8 +501,11 @@
       <c r="D1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -510,8 +518,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -524,8 +535,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -538,8 +552,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -552,8 +569,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -566,8 +586,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -580,8 +603,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -594,8 +620,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -608,8 +637,11 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -622,8 +654,11 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -636,8 +671,11 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -650,8 +688,11 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -664,8 +705,11 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -678,8 +722,11 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -692,8 +739,11 @@
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -706,8 +756,11 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -720,8 +773,11 @@
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -732,6 +788,9 @@
         <v>3</v>
       </c>
       <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
         <v>1</v>
       </c>
     </row>
@@ -745,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5005D96F-105D-4071-A89A-95B155F84A28}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
actor 테이블에 attackRange, ultimateRange 추가
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F64486-7A3A-406B-B662-5D8A88E0F787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD50F4E5-8308-4737-87CA-D99C3EC76A0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
   <sheets>
     <sheet name="ActorTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
   <si>
     <t>Actor002</t>
   </si>
@@ -125,6 +125,14 @@
   </si>
   <si>
     <t>Actor003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackRange|Float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ultimateRange|Float</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -492,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAEF85E-644F-4CA8-8208-63C893B0C10A}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -503,7 +511,7 @@
     <col min="4" max="4" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -525,8 +533,14 @@
       <c r="G1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -548,8 +562,14 @@
       <c r="G2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -571,8 +591,14 @@
       <c r="G3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -594,8 +620,14 @@
       <c r="G4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -617,8 +649,14 @@
       <c r="G5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -640,8 +678,14 @@
       <c r="G6">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -663,8 +707,14 @@
       <c r="G7">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -686,8 +736,14 @@
       <c r="G8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -709,8 +765,14 @@
       <c r="G9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -732,8 +794,14 @@
       <c r="G10">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -755,8 +823,14 @@
       <c r="G11">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -778,8 +852,14 @@
       <c r="G12">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -801,8 +881,14 @@
       <c r="G13">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -824,8 +910,14 @@
       <c r="G14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -847,8 +939,14 @@
       <c r="G15">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -870,8 +968,14 @@
       <c r="G16">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -893,8 +997,14 @@
       <c r="G17">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -915,6 +1025,12 @@
       </c>
       <c r="G18">
         <v>30</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
액터테이블 컬럼명 변경 multiAtkVisual => multiAtk
어펙터밸류 배율 수치 조정
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB18496E-66B3-49F9-9D5A-3E2A348EEA4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055419F6-2F4E-4026-8F2B-DB39520FDB72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
@@ -117,7 +117,7 @@
     <t>multiHp|Float</t>
   </si>
   <si>
-    <t>multiAtkVisual|Float</t>
+    <t>multiAtk|Float</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
         <v>0.85</v>
       </c>
       <c r="D3">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>

<commit_message>
액터 테이블에 portaitAddress|String 추가
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01588916-92B8-4555-BF08-7F76B7709BBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778CD1C9-0CC0-48D7-873D-12C92C51B929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Actor002</t>
   </si>
@@ -164,6 +164,21 @@
   </si>
   <si>
     <t>CharDesc_Bei</t>
+  </si>
+  <si>
+    <t>portraitAddress|String</t>
+  </si>
+  <si>
+    <t>Portrati_Ganfaul</t>
+  </si>
+  <si>
+    <t>Portrati_KeepSeries</t>
+  </si>
+  <si>
+    <t>Portrati_BigBatSuccubus</t>
+  </si>
+  <si>
+    <t>Portrati_Bei</t>
   </si>
 </sst>
 </file>
@@ -530,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAEF85E-644F-4CA8-8208-63C893B0C10A}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -539,9 +554,10 @@
     <col min="1" max="3" width="12.5" customWidth="1"/>
     <col min="7" max="7" width="16.375" customWidth="1"/>
     <col min="12" max="12" width="19.25" customWidth="1"/>
+    <col min="13" max="13" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -578,8 +594,11 @@
       <c r="L1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -616,8 +635,11 @@
       <c r="L2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -654,8 +676,11 @@
       <c r="L3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -692,8 +717,11 @@
       <c r="L4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -730,8 +758,11 @@
       <c r="L5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -760,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -789,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -818,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -847,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -876,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -905,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -934,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -963,7 +994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -992,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1021,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
빅뱃 공속 조절 0.7 => 0.77
액터테이블에 flying|Bool 컬럼 추가

젤리피쉬걸 테이블 등록
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0492C72-8473-4FBB-8374-7E228350DCDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BF97FD-D6EF-4832-8751-44840CBB0257}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
   <sheets>
     <sheet name="ActorTable" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Actor002</t>
   </si>
@@ -182,6 +182,21 @@
   </si>
   <si>
     <t>targetingSphereRadius|Float</t>
+  </si>
+  <si>
+    <t>flying|Bool</t>
+  </si>
+  <si>
+    <t>CharName_JellyFishGirl</t>
+  </si>
+  <si>
+    <t>CharDesc_JellyFishGirl</t>
+  </si>
+  <si>
+    <t>JellyFishGirl</t>
+  </si>
+  <si>
+    <t>Portrait_JellyFishGirl</t>
   </si>
 </sst>
 </file>
@@ -548,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAEF85E-644F-4CA8-8208-63C893B0C10A}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -560,7 +575,7 @@
     <col min="13" max="13" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -603,8 +618,11 @@
       <c r="N1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -621,7 +639,7 @@
         <v>0.95</v>
       </c>
       <c r="F2">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="G2">
         <v>0.7</v>
@@ -647,8 +665,11 @@
       <c r="N2">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -691,8 +712,11 @@
       <c r="N3">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -712,7 +736,7 @@
         <v>0.9</v>
       </c>
       <c r="G4">
-        <v>0.7</v>
+        <v>0.77</v>
       </c>
       <c r="H4">
         <v>3.5</v>
@@ -735,8 +759,11 @@
       <c r="N4">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -779,28 +806,37 @@
       <c r="N5">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.87</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0.82</v>
       </c>
       <c r="G6">
-        <v>0.7</v>
+        <v>0.83</v>
       </c>
       <c r="H6">
         <v>3.5</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>100</v>
@@ -808,8 +844,20 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6">
+        <v>0.05</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -837,8 +885,11 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -866,8 +917,11 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -895,8 +949,11 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -924,8 +981,11 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -953,8 +1013,11 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -982,8 +1045,11 @@
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1011,8 +1077,11 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1040,8 +1109,11 @@
       <c r="K14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1069,8 +1141,11 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1098,8 +1173,11 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1127,8 +1205,11 @@
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1154,6 +1235,9 @@
         <v>100</v>
       </c>
       <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actor009	SciFiWarrior Actor010	ChaosElemental Actor011	SuperHero Actor012	Meryl Actor013	GreekWarrior
액터 테이블 추가
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AC102C-75F7-494B-AFFE-FB88C2CCD44E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD898866-33CE-439A-8A2A-4EB2C339BB67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
   <sheets>
     <sheet name="ActorTable" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Actor002</t>
   </si>
@@ -233,6 +233,66 @@
   </si>
   <si>
     <t>Portrait_DynaMob</t>
+  </si>
+  <si>
+    <t>CharName_SciFiWarrior</t>
+  </si>
+  <si>
+    <t>CharDesc_SciFiWarrior</t>
+  </si>
+  <si>
+    <t>SciFiWarrior</t>
+  </si>
+  <si>
+    <t>Portrait_SciFiWarrior</t>
+  </si>
+  <si>
+    <t>CharName_ChaosElemental</t>
+  </si>
+  <si>
+    <t>CharDesc_ChaosElemental</t>
+  </si>
+  <si>
+    <t>ChaosElemental</t>
+  </si>
+  <si>
+    <t>Portrait_ChaosElemental</t>
+  </si>
+  <si>
+    <t>CharName_SuperHero</t>
+  </si>
+  <si>
+    <t>CharDesc_SuperHero</t>
+  </si>
+  <si>
+    <t>SuperHero</t>
+  </si>
+  <si>
+    <t>Portrait_SuperHero</t>
+  </si>
+  <si>
+    <t>CharName_Meryl</t>
+  </si>
+  <si>
+    <t>CharDesc_Meryl</t>
+  </si>
+  <si>
+    <t>Meryl</t>
+  </si>
+  <si>
+    <t>Portrait_Meryl</t>
+  </si>
+  <si>
+    <t>CharName_GreekWarrior</t>
+  </si>
+  <si>
+    <t>CharDesc_GreekWarrior</t>
+  </si>
+  <si>
+    <t>GreekWarrior</t>
+  </si>
+  <si>
+    <t>Portrait_GreekWarrior</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1098,14 @@
       <c r="A10" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1054,13 +1120,22 @@
         <v>3.5</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>50</v>
       </c>
       <c r="K10">
         <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10">
+        <v>0.05</v>
       </c>
       <c r="O10" t="b">
         <v>0</v>
@@ -1070,6 +1145,12 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
       <c r="D11">
         <v>0</v>
       </c>
@@ -1086,7 +1167,7 @@
         <v>3.5</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11">
         <v>50</v>
@@ -1094,14 +1175,29 @@
       <c r="K11">
         <v>0</v>
       </c>
+      <c r="L11" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11">
+        <v>0.05</v>
+      </c>
       <c r="O11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
       <c r="D12">
         <v>0</v>
       </c>
@@ -1125,6 +1221,15 @@
       </c>
       <c r="K12">
         <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M12" t="s">
+        <v>78</v>
+      </c>
+      <c r="N12">
+        <v>0.05</v>
       </c>
       <c r="O12" t="b">
         <v>0</v>
@@ -1134,8 +1239,14 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1150,13 +1261,22 @@
         <v>3.5</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>50</v>
       </c>
       <c r="K13">
         <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>81</v>
+      </c>
+      <c r="M13" t="s">
+        <v>82</v>
+      </c>
+      <c r="N13">
+        <v>0.05</v>
       </c>
       <c r="O13" t="b">
         <v>0</v>
@@ -1166,8 +1286,14 @@
       <c r="A14" t="s">
         <v>11</v>
       </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1189,6 +1315,15 @@
       </c>
       <c r="K14">
         <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>85</v>
+      </c>
+      <c r="M14" t="s">
+        <v>86</v>
+      </c>
+      <c r="N14">
+        <v>0.05</v>
       </c>
       <c r="O14" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
신규 3종 캐릭터 테이블 추가 14 Akai 15 Yuka 16 SteampunkRobot
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD898866-33CE-439A-8A2A-4EB2C339BB67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD892E6D-9F50-4ED9-B4BA-696E503AE438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>Actor002</t>
   </si>
@@ -293,6 +293,42 @@
   </si>
   <si>
     <t>Portrait_GreekWarrior</t>
+  </si>
+  <si>
+    <t>Akai</t>
+  </si>
+  <si>
+    <t>Yuka</t>
+  </si>
+  <si>
+    <t>SteampunkRobot</t>
+  </si>
+  <si>
+    <t>CharName_Akai</t>
+  </si>
+  <si>
+    <t>CharDesc_Akai</t>
+  </si>
+  <si>
+    <t>Portrait_Akai</t>
+  </si>
+  <si>
+    <t>CharName_Yuka</t>
+  </si>
+  <si>
+    <t>CharDesc_Yuka</t>
+  </si>
+  <si>
+    <t>Portrait_Yuka</t>
+  </si>
+  <si>
+    <t>CharName_SteampunkRobot</t>
+  </si>
+  <si>
+    <t>CharDesc_SteampunkRobot</t>
+  </si>
+  <si>
+    <t>Portrait_SteampunkRobot</t>
   </si>
 </sst>
 </file>
@@ -1333,8 +1369,14 @@
       <c r="A15" t="s">
         <v>12</v>
       </c>
+      <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1349,13 +1391,19 @@
         <v>3.5</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J15">
         <v>50</v>
       </c>
       <c r="K15">
         <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M15" t="s">
+        <v>92</v>
       </c>
       <c r="O15" t="b">
         <v>0</v>
@@ -1365,8 +1413,14 @@
       <c r="A16" t="s">
         <v>13</v>
       </c>
+      <c r="B16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1381,13 +1435,19 @@
         <v>3.5</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>50</v>
       </c>
       <c r="K16">
         <v>0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>88</v>
+      </c>
+      <c r="M16" t="s">
+        <v>95</v>
       </c>
       <c r="O16" t="b">
         <v>0</v>
@@ -1397,6 +1457,12 @@
       <c r="A17" t="s">
         <v>14</v>
       </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
       <c r="D17">
         <v>0</v>
       </c>
@@ -1413,13 +1479,19 @@
         <v>3.5</v>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J17">
         <v>50</v>
       </c>
       <c r="K17">
         <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17" t="s">
+        <v>98</v>
       </c>
       <c r="O17" t="b">
         <v>0</v>
@@ -1460,6 +1532,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SP 50 => 75 조정
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DCC563-2589-4876-B0CC-BE7B72E42D81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F7BF36-509B-45DE-AD54-726C115D5C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
   <sheets>
     <sheet name="ActorTable" sheetId="1" r:id="rId1"/>
@@ -1079,7 +1079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAEF85E-644F-4CA8-8208-63C893B0C10A}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1165,7 +1165,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1212,7 +1212,7 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1259,7 +1259,7 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K4">
         <v>8</v>
@@ -1306,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K5">
         <v>5</v>
@@ -1353,7 +1353,7 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1400,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1447,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1494,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K9">
         <v>4</v>
@@ -1541,7 +1541,7 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1588,7 +1588,7 @@
         <v>2</v>
       </c>
       <c r="J11">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1635,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="J12">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1682,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1729,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1776,7 +1776,7 @@
         <v>3</v>
       </c>
       <c r="J15">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -1823,7 +1823,7 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -1870,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1917,7 +1917,7 @@
         <v>3</v>
       </c>
       <c r="J18">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1964,7 +1964,7 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -2011,7 +2011,7 @@
         <v>3</v>
       </c>
       <c r="J20">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -2058,7 +2058,7 @@
         <v>2</v>
       </c>
       <c r="J21">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -2105,7 +2105,7 @@
         <v>3</v>
       </c>
       <c r="J22">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -2152,7 +2152,7 @@
         <v>3</v>
       </c>
       <c r="J23">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -2199,7 +2199,7 @@
         <v>2</v>
       </c>
       <c r="J24">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -2246,7 +2246,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -2293,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -2340,7 +2340,7 @@
         <v>1</v>
       </c>
       <c r="J27">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -2387,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="J28">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -2434,7 +2434,7 @@
         <v>1</v>
       </c>
       <c r="J29">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -2481,7 +2481,7 @@
         <v>1</v>
       </c>
       <c r="J30">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -2528,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -2575,7 +2575,7 @@
         <v>3</v>
       </c>
       <c r="J32">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -2622,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -2669,7 +2669,7 @@
         <v>3</v>
       </c>
       <c r="J34">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -2716,7 +2716,7 @@
         <v>1</v>
       </c>
       <c r="J35">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -2763,7 +2763,7 @@
         <v>2</v>
       </c>
       <c r="J36">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -2857,7 +2857,7 @@
         <v>0</v>
       </c>
       <c r="J38">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -2904,7 +2904,7 @@
         <v>2</v>
       </c>
       <c r="J39">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -2951,7 +2951,7 @@
         <v>1</v>
       </c>
       <c r="J40">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -2998,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -3042,10 +3042,10 @@
         <v>3.5</v>
       </c>
       <c r="I42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J42">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -3074,7 +3074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151E6CB5-8C53-40F7-9E93-03CEE2EEECC6}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
파워레벨 테이블에 requiredLimitBreakGold|Int 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49093CB6-DCD7-407C-A085-F4E5E939B1A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C0B4EB-4DB0-4597-8CFB-131A0E44CD93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
   <sheets>
     <sheet name="ActorTable" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="282">
   <si>
     <t>Actor002</t>
   </si>
@@ -876,6 +876,9 @@
   </si>
   <si>
     <t>requiredGold|Int</t>
+  </si>
+  <si>
+    <t>requiredLimitBreakGold|Int</t>
   </si>
 </sst>
 </file>
@@ -3603,10 +3606,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5005D96F-105D-4071-A89A-95B155F84A28}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3614,7 +3617,7 @@
     <col min="1" max="1" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -3628,16 +3631,19 @@
         <v>277</v>
       </c>
       <c r="E1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F1" t="s">
         <v>278</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>279</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3659,8 +3665,11 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3674,16 +3683,19 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>20</v>
       </c>
       <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3697,16 +3709,19 @@
         <v>0</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>30</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>50</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>3500</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3720,16 +3735,19 @@
         <v>0</v>
       </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>50</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>100</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>7500</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3743,16 +3761,19 @@
         <v>0</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>70</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>170</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>14000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3766,16 +3787,19 @@
         <v>0</v>
       </c>
       <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>90</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>260</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>29000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3789,16 +3813,19 @@
         <v>0</v>
       </c>
       <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>120</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>380</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>48000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3812,16 +3839,19 @@
         <v>0</v>
       </c>
       <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>170</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>550</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>80000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3835,16 +3865,19 @@
         <v>0</v>
       </c>
       <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>240</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>790</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>125000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3858,16 +3891,19 @@
         <v>0</v>
       </c>
       <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>330</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1120</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>150000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3881,16 +3917,19 @@
         <v>1</v>
       </c>
       <c r="E12">
+        <v>270000</v>
+      </c>
+      <c r="F12">
         <v>450</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1570</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>180000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3904,16 +3943,19 @@
         <v>1</v>
       </c>
       <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
         <v>620</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>2190</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>220000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3927,16 +3969,19 @@
         <v>1</v>
       </c>
       <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
         <v>860</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>3050</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>260000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3950,16 +3995,19 @@
         <v>2</v>
       </c>
       <c r="E15">
+        <v>465000</v>
+      </c>
+      <c r="F15">
         <v>1190</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>4240</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>310000</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3973,16 +4021,19 @@
         <v>2</v>
       </c>
       <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>1640</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>5880</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>370000</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3996,16 +4047,19 @@
         <v>2</v>
       </c>
       <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
         <v>2260</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>8140</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>440000</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4019,16 +4073,19 @@
         <v>3</v>
       </c>
       <c r="E18">
+        <v>795000</v>
+      </c>
+      <c r="F18">
         <v>3120</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>11260</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>530000</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4042,16 +4099,19 @@
         <v>3</v>
       </c>
       <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
         <v>4310</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>15570</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>640000</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4065,16 +4125,19 @@
         <v>3</v>
       </c>
       <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
         <v>5950</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>21520</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>770000</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4088,12 +4151,15 @@
         <v>3</v>
       </c>
       <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>8210</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>29730</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>920000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ActorTable 에 battltMusicOverriding|String 컬럼 추가 ChapterTable 에 chapterMusic|String 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53E2CF2-D287-4B95-9480-69854413427B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C98EBC-AB44-4E61-831A-0C7D65B4E5E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
   <sheets>
     <sheet name="ActorTable" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="408">
   <si>
     <t>actorId|String</t>
   </si>
@@ -1402,6 +1402,9 @@
   </si>
   <si>
     <t>Wing_WhiteFullNoiseOtherFast</t>
+  </si>
+  <si>
+    <t>battltMusicOverriding|String</t>
   </si>
 </sst>
 </file>
@@ -1792,11 +1795,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAEF85E-644F-4CA8-8208-63C893B0C10A}">
-  <dimension ref="A1:AB37"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1806,7 +1807,7 @@
     <col min="15" max="15" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1889,10 +1890,13 @@
         <v>296</v>
       </c>
       <c r="AB1" t="s">
+        <v>407</v>
+      </c>
+      <c r="AC1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>246</v>
       </c>
@@ -1974,11 +1978,11 @@
       <c r="AA2">
         <v>151</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>247</v>
       </c>
@@ -2060,11 +2064,11 @@
       <c r="AA3">
         <v>245</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>267</v>
       </c>
@@ -2146,11 +2150,11 @@
       <c r="AA4">
         <v>204</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>248</v>
       </c>
@@ -2232,11 +2236,11 @@
       <c r="AA5">
         <v>151</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>249</v>
       </c>
@@ -2318,11 +2322,11 @@
       <c r="AA6">
         <v>234</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>268</v>
       </c>
@@ -2404,11 +2408,11 @@
       <c r="AA7">
         <v>151</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -2490,11 +2494,11 @@
       <c r="AA8">
         <v>151</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>269</v>
       </c>
@@ -2576,11 +2580,11 @@
       <c r="AA9">
         <v>151</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -2662,11 +2666,11 @@
       <c r="AA10">
         <v>151</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>252</v>
       </c>
@@ -2748,11 +2752,11 @@
       <c r="AA11">
         <v>151</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>253</v>
       </c>
@@ -2834,11 +2838,11 @@
       <c r="AA12">
         <v>151</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>254</v>
       </c>
@@ -2920,11 +2924,11 @@
       <c r="AA13">
         <v>151</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>270</v>
       </c>
@@ -3006,11 +3010,11 @@
       <c r="AA14">
         <v>151</v>
       </c>
-      <c r="AB14">
+      <c r="AC14">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>271</v>
       </c>
@@ -3092,11 +3096,11 @@
       <c r="AA15">
         <v>151</v>
       </c>
-      <c r="AB15">
+      <c r="AC15">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>272</v>
       </c>
@@ -3178,11 +3182,11 @@
       <c r="AA16">
         <v>151</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>255</v>
       </c>
@@ -3264,11 +3268,11 @@
       <c r="AA17">
         <v>151</v>
       </c>
-      <c r="AB17">
+      <c r="AC17">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>256</v>
       </c>
@@ -3350,11 +3354,11 @@
       <c r="AA18">
         <v>151</v>
       </c>
-      <c r="AB18">
+      <c r="AC18">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>257</v>
       </c>
@@ -3436,11 +3440,11 @@
       <c r="AA19">
         <v>151</v>
       </c>
-      <c r="AB19">
+      <c r="AC19">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>258</v>
       </c>
@@ -3522,11 +3526,11 @@
       <c r="AA20">
         <v>151</v>
       </c>
-      <c r="AB20">
+      <c r="AC20">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>259</v>
       </c>
@@ -3608,11 +3612,11 @@
       <c r="AA21">
         <v>151</v>
       </c>
-      <c r="AB21">
+      <c r="AC21">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>273</v>
       </c>
@@ -3694,11 +3698,11 @@
       <c r="AA22">
         <v>151</v>
       </c>
-      <c r="AB22">
+      <c r="AC22">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>274</v>
       </c>
@@ -3780,11 +3784,11 @@
       <c r="AA23">
         <v>151</v>
       </c>
-      <c r="AB23">
+      <c r="AC23">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>275</v>
       </c>
@@ -3866,11 +3870,11 @@
       <c r="AA24">
         <v>151</v>
       </c>
-      <c r="AB24">
+      <c r="AC24">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>276</v>
       </c>
@@ -3952,11 +3956,11 @@
       <c r="AA25">
         <v>151</v>
       </c>
-      <c r="AB25">
+      <c r="AC25">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>277</v>
       </c>
@@ -4038,11 +4042,11 @@
       <c r="AA26">
         <v>151</v>
       </c>
-      <c r="AB26">
+      <c r="AC26">
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>278</v>
       </c>
@@ -4124,11 +4128,11 @@
       <c r="AA27">
         <v>151</v>
       </c>
-      <c r="AB27">
+      <c r="AC27">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>260</v>
       </c>
@@ -4210,11 +4214,11 @@
       <c r="AA28">
         <v>151</v>
       </c>
-      <c r="AB28">
+      <c r="AC28">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>279</v>
       </c>
@@ -4296,11 +4300,11 @@
       <c r="AA29">
         <v>151</v>
       </c>
-      <c r="AB29">
+      <c r="AC29">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>261</v>
       </c>
@@ -4382,11 +4386,11 @@
       <c r="AA30">
         <v>151</v>
       </c>
-      <c r="AB30">
+      <c r="AC30">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>262</v>
       </c>
@@ -4468,11 +4472,11 @@
       <c r="AA31">
         <v>151</v>
       </c>
-      <c r="AB31">
+      <c r="AC31">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>263</v>
       </c>
@@ -4554,11 +4558,11 @@
       <c r="AA32">
         <v>151</v>
       </c>
-      <c r="AB32">
+      <c r="AC32">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>280</v>
       </c>
@@ -4640,11 +4644,11 @@
       <c r="AA33">
         <v>151</v>
       </c>
-      <c r="AB33">
+      <c r="AC33">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>281</v>
       </c>
@@ -4726,11 +4730,11 @@
       <c r="AA34">
         <v>151</v>
       </c>
-      <c r="AB34">
+      <c r="AC34">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>264</v>
       </c>
@@ -4812,11 +4816,11 @@
       <c r="AA35">
         <v>151</v>
       </c>
-      <c r="AB35">
+      <c r="AC35">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>265</v>
       </c>
@@ -4898,11 +4902,11 @@
       <c r="AA36">
         <v>151</v>
       </c>
-      <c r="AB36">
+      <c r="AC36">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>266</v>
       </c>
@@ -4984,7 +4988,7 @@
       <c r="AA37">
         <v>151</v>
       </c>
-      <c r="AB37">
+      <c r="AC37">
         <v>85</v>
       </c>
     </row>
@@ -5898,7 +5902,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5906,7 +5910,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5914,7 +5918,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5922,7 +5926,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -6246,7 +6250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59613FA1-939D-46DB-A7F6-72F2ABB4CE9A}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
attackHitObjectRange|Float 컬럼 추가하고 시리아 설정
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C754366-02D6-4A35-A4D5-D0750F07F801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F2C220-0B62-45CD-8E86-6C597A583254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="410">
   <si>
     <t>actorId|String</t>
   </si>
@@ -1408,6 +1408,9 @@
   </si>
   <si>
     <t>multiTargetAngle|Float</t>
+  </si>
+  <si>
+    <t>attackHitObjectRange|Float</t>
   </si>
 </sst>
 </file>
@@ -1798,21 +1801,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAEF85E-644F-4CA8-8208-63C893B0C10A}">
-  <dimension ref="A1:AD37"/>
+  <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="5" width="12.5" customWidth="1"/>
     <col min="9" max="9" width="16.375" customWidth="1"/>
-    <col min="14" max="14" width="19.25" customWidth="1"/>
-    <col min="15" max="15" width="17.625" customWidth="1"/>
+    <col min="16" max="16" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1856,55 +1856,58 @@
         <v>408</v>
       </c>
       <c r="O1" t="s">
+        <v>409</v>
+      </c>
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>203</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>282</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>289</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>290</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>291</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>292</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>293</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>294</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>295</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>296</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>407</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>246</v>
       </c>
@@ -1947,53 +1950,56 @@
       <c r="N2">
         <v>0</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>28</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.05</v>
       </c>
-      <c r="R2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
+      <c r="S2" t="b">
+        <v>0</v>
       </c>
       <c r="T2">
         <v>1</v>
       </c>
       <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
         <v>13</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>11</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>9</v>
       </c>
-      <c r="X2">
-        <v>10</v>
-      </c>
       <c r="Y2">
+        <v>10</v>
+      </c>
+      <c r="Z2">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>119</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>151</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>247</v>
       </c>
@@ -2036,53 +2042,56 @@
       <c r="N3">
         <v>0</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
         <v>14</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0.25</v>
       </c>
-      <c r="R3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3">
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3">
         <v>45</v>
       </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
       <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
         <v>9</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>12</v>
       </c>
-      <c r="W3">
-        <v>10</v>
-      </c>
       <c r="X3">
+        <v>10</v>
+      </c>
+      <c r="Y3">
         <v>8</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>0.16470000000000001</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>0.1024</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>151</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>245</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>267</v>
       </c>
@@ -2125,53 +2134,56 @@
       <c r="N4">
         <v>0</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
         <v>15</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>30</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.15</v>
       </c>
-      <c r="R4" t="b">
-        <v>0</v>
-      </c>
-      <c r="S4">
+      <c r="S4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4">
         <v>27</v>
       </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
       <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
         <v>11</v>
       </c>
-      <c r="V4">
-        <v>10</v>
-      </c>
       <c r="W4">
+        <v>10</v>
+      </c>
+      <c r="X4">
         <v>11</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>9</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>0.20150000000000001</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>0.13239999999999999</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>125</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>204</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>248</v>
       </c>
@@ -2214,26 +2226,26 @@
       <c r="N5">
         <v>0</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
         <v>16</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>31</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.2</v>
       </c>
-      <c r="R5" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5">
+      <c r="S5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5">
         <v>22</v>
       </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
       <c r="U5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V5">
         <v>10</v>
@@ -2245,22 +2257,25 @@
         <v>10</v>
       </c>
       <c r="Y5">
+        <v>10</v>
+      </c>
+      <c r="Z5">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>119</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>151</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>249</v>
       </c>
@@ -2303,53 +2318,56 @@
       <c r="N6">
         <v>0</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
         <v>36</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>37</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6">
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="b">
+        <v>0</v>
+      </c>
+      <c r="T6">
         <v>47</v>
       </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
       <c r="U6">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <v>9</v>
       </c>
       <c r="W6">
+        <v>9</v>
+      </c>
+      <c r="X6">
         <v>11</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>8</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>0.15179999999999999</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>0.12239999999999999</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>145</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>234</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>268</v>
       </c>
@@ -2392,26 +2410,26 @@
       <c r="N7">
         <v>0</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
         <v>40</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>41</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>0.15</v>
       </c>
-      <c r="R7" t="b">
-        <v>0</v>
-      </c>
-      <c r="S7">
+      <c r="S7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7">
         <v>43</v>
       </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
       <c r="U7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <v>10</v>
@@ -2423,22 +2441,25 @@
         <v>10</v>
       </c>
       <c r="Y7">
+        <v>10</v>
+      </c>
+      <c r="Z7">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>119</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>151</v>
       </c>
-      <c r="AD7">
+      <c r="AE7">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -2481,26 +2502,26 @@
       <c r="N8">
         <v>180</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
         <v>44</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>45</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8" t="b">
-        <v>0</v>
-      </c>
-      <c r="S8">
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" t="b">
+        <v>0</v>
+      </c>
+      <c r="T8">
         <v>24</v>
       </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
       <c r="U8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <v>10</v>
@@ -2512,22 +2533,25 @@
         <v>10</v>
       </c>
       <c r="Y8">
+        <v>10</v>
+      </c>
+      <c r="Z8">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <v>119</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <v>151</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>269</v>
       </c>
@@ -2570,26 +2594,26 @@
       <c r="N9">
         <v>0</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
         <v>48</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>49</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>0.05</v>
       </c>
-      <c r="R9" t="b">
-        <v>0</v>
-      </c>
-      <c r="S9">
+      <c r="S9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9">
         <v>26</v>
       </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
       <c r="U9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <v>10</v>
@@ -2601,22 +2625,25 @@
         <v>10</v>
       </c>
       <c r="Y9">
+        <v>10</v>
+      </c>
+      <c r="Z9">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>119</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>151</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -2659,26 +2686,26 @@
       <c r="N10">
         <v>0</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
         <v>52</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>53</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>0.1</v>
       </c>
-      <c r="R10" t="b">
-        <v>1</v>
-      </c>
-      <c r="S10">
+      <c r="S10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10">
         <v>49</v>
       </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
       <c r="U10">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V10">
         <v>10</v>
@@ -2690,22 +2717,25 @@
         <v>10</v>
       </c>
       <c r="Y10">
+        <v>10</v>
+      </c>
+      <c r="Z10">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>119</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <v>151</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>252</v>
       </c>
@@ -2748,26 +2778,26 @@
       <c r="N11">
         <v>0</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
         <v>56</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>57</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>0.05</v>
       </c>
-      <c r="R11" t="b">
-        <v>0</v>
-      </c>
-      <c r="S11">
+      <c r="S11" t="b">
+        <v>0</v>
+      </c>
+      <c r="T11">
         <v>51</v>
       </c>
-      <c r="T11">
-        <v>1</v>
-      </c>
       <c r="U11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V11">
         <v>10</v>
@@ -2779,22 +2809,25 @@
         <v>10</v>
       </c>
       <c r="Y11">
+        <v>10</v>
+      </c>
+      <c r="Z11">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>119</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>151</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>253</v>
       </c>
@@ -2837,26 +2870,26 @@
       <c r="N12">
         <v>0</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
         <v>60</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>61</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>0.05</v>
       </c>
-      <c r="R12" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>10</v>
+      <c r="S12" t="b">
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V12">
         <v>10</v>
@@ -2868,22 +2901,25 @@
         <v>10</v>
       </c>
       <c r="Y12">
+        <v>10</v>
+      </c>
+      <c r="Z12">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>119</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <v>151</v>
       </c>
-      <c r="AD12">
+      <c r="AE12">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>254</v>
       </c>
@@ -2926,26 +2962,26 @@
       <c r="N13">
         <v>0</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
         <v>64</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>65</v>
       </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13" t="b">
-        <v>0</v>
-      </c>
-      <c r="S13">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13" t="b">
+        <v>0</v>
+      </c>
+      <c r="T13">
         <v>21</v>
       </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
       <c r="U13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V13">
         <v>10</v>
@@ -2957,22 +2993,25 @@
         <v>10</v>
       </c>
       <c r="Y13">
+        <v>10</v>
+      </c>
+      <c r="Z13">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>119</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <v>151</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>270</v>
       </c>
@@ -3015,26 +3054,26 @@
       <c r="N14">
         <v>0</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
         <v>66</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>71</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>0.05</v>
       </c>
-      <c r="R14" t="b">
-        <v>0</v>
-      </c>
-      <c r="S14">
+      <c r="S14" t="b">
+        <v>0</v>
+      </c>
+      <c r="T14">
         <v>30</v>
       </c>
-      <c r="T14">
-        <v>1</v>
-      </c>
       <c r="U14">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <v>10</v>
@@ -3046,22 +3085,25 @@
         <v>10</v>
       </c>
       <c r="Y14">
+        <v>10</v>
+      </c>
+      <c r="Z14">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <v>119</v>
       </c>
-      <c r="AB14">
+      <c r="AC14">
         <v>151</v>
       </c>
-      <c r="AD14">
+      <c r="AE14">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>271</v>
       </c>
@@ -3104,26 +3146,26 @@
       <c r="N15">
         <v>0</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
         <v>67</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>74</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>0.05</v>
       </c>
-      <c r="R15" t="b">
-        <v>0</v>
-      </c>
-      <c r="S15">
+      <c r="S15" t="b">
+        <v>0</v>
+      </c>
+      <c r="T15">
         <v>50</v>
       </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
       <c r="U15">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V15">
         <v>10</v>
@@ -3135,22 +3177,25 @@
         <v>10</v>
       </c>
       <c r="Y15">
+        <v>10</v>
+      </c>
+      <c r="Z15">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z15">
+      <c r="AA15">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <v>119</v>
       </c>
-      <c r="AB15">
+      <c r="AC15">
         <v>151</v>
       </c>
-      <c r="AD15">
+      <c r="AE15">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>272</v>
       </c>
@@ -3193,26 +3238,26 @@
       <c r="N16">
         <v>0</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
         <v>68</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>77</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>0.05</v>
       </c>
-      <c r="R16" t="b">
-        <v>0</v>
-      </c>
-      <c r="S16">
+      <c r="S16" t="b">
+        <v>0</v>
+      </c>
+      <c r="T16">
         <v>5</v>
       </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
       <c r="U16">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V16">
         <v>10</v>
@@ -3224,22 +3269,25 @@
         <v>10</v>
       </c>
       <c r="Y16">
+        <v>10</v>
+      </c>
+      <c r="Z16">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z16">
+      <c r="AA16">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <v>119</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <v>151</v>
       </c>
-      <c r="AD16">
+      <c r="AE16">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>255</v>
       </c>
@@ -3282,26 +3330,26 @@
       <c r="N17">
         <v>0</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
         <v>80</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>81</v>
       </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17" t="b">
-        <v>0</v>
-      </c>
-      <c r="S17">
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" t="b">
+        <v>0</v>
+      </c>
+      <c r="T17">
         <v>31</v>
       </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
       <c r="U17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V17">
         <v>10</v>
@@ -3313,22 +3361,25 @@
         <v>10</v>
       </c>
       <c r="Y17">
+        <v>10</v>
+      </c>
+      <c r="Z17">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z17">
+      <c r="AA17">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <v>119</v>
       </c>
-      <c r="AB17">
+      <c r="AC17">
         <v>151</v>
       </c>
-      <c r="AD17">
+      <c r="AE17">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>256</v>
       </c>
@@ -3371,26 +3422,26 @@
       <c r="N18">
         <v>360</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
         <v>84</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>85</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>0.05</v>
       </c>
-      <c r="R18" t="b">
-        <v>0</v>
-      </c>
-      <c r="S18">
+      <c r="S18" t="b">
+        <v>0</v>
+      </c>
+      <c r="T18">
         <v>6</v>
       </c>
-      <c r="T18">
-        <v>1</v>
-      </c>
       <c r="U18">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V18">
         <v>10</v>
@@ -3402,22 +3453,25 @@
         <v>10</v>
       </c>
       <c r="Y18">
+        <v>10</v>
+      </c>
+      <c r="Z18">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z18">
+      <c r="AA18">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA18">
+      <c r="AB18">
         <v>119</v>
       </c>
-      <c r="AB18">
+      <c r="AC18">
         <v>151</v>
       </c>
-      <c r="AD18">
+      <c r="AE18">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>257</v>
       </c>
@@ -3460,26 +3514,26 @@
       <c r="N19">
         <v>0</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
         <v>88</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>89</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>0.2</v>
       </c>
-      <c r="R19" t="b">
-        <v>0</v>
-      </c>
-      <c r="S19">
+      <c r="S19" t="b">
+        <v>0</v>
+      </c>
+      <c r="T19">
         <v>53</v>
       </c>
-      <c r="T19">
-        <v>1</v>
-      </c>
       <c r="U19">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V19">
         <v>10</v>
@@ -3491,22 +3545,25 @@
         <v>10</v>
       </c>
       <c r="Y19">
+        <v>10</v>
+      </c>
+      <c r="Z19">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z19">
+      <c r="AA19">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA19">
+      <c r="AB19">
         <v>119</v>
       </c>
-      <c r="AB19">
+      <c r="AC19">
         <v>151</v>
       </c>
-      <c r="AD19">
+      <c r="AE19">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>258</v>
       </c>
@@ -3549,26 +3606,26 @@
       <c r="N20">
         <v>0</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20" t="s">
         <v>92</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>93</v>
       </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20" t="b">
-        <v>0</v>
-      </c>
-      <c r="S20">
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20" t="b">
+        <v>0</v>
+      </c>
+      <c r="T20">
         <v>28</v>
       </c>
-      <c r="T20">
-        <v>1</v>
-      </c>
       <c r="U20">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V20">
         <v>10</v>
@@ -3580,22 +3637,25 @@
         <v>10</v>
       </c>
       <c r="Y20">
+        <v>10</v>
+      </c>
+      <c r="Z20">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z20">
+      <c r="AA20">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA20">
+      <c r="AB20">
         <v>119</v>
       </c>
-      <c r="AB20">
+      <c r="AC20">
         <v>151</v>
       </c>
-      <c r="AD20">
+      <c r="AE20">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>259</v>
       </c>
@@ -3638,26 +3698,26 @@
       <c r="N21">
         <v>0</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
         <v>96</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>97</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R21" t="b">
-        <v>0</v>
-      </c>
-      <c r="S21">
+      <c r="S21" t="b">
+        <v>0</v>
+      </c>
+      <c r="T21">
         <v>52</v>
       </c>
-      <c r="T21">
-        <v>1</v>
-      </c>
       <c r="U21">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V21">
         <v>10</v>
@@ -3669,22 +3729,25 @@
         <v>10</v>
       </c>
       <c r="Y21">
+        <v>10</v>
+      </c>
+      <c r="Z21">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z21">
+      <c r="AA21">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA21">
+      <c r="AB21">
         <v>119</v>
       </c>
-      <c r="AB21">
+      <c r="AC21">
         <v>151</v>
       </c>
-      <c r="AD21">
+      <c r="AE21">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>273</v>
       </c>
@@ -3727,26 +3790,26 @@
       <c r="N22">
         <v>0</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
         <v>100</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>101</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>0.12</v>
       </c>
-      <c r="R22" t="b">
-        <v>0</v>
-      </c>
-      <c r="S22">
+      <c r="S22" t="b">
+        <v>0</v>
+      </c>
+      <c r="T22">
         <v>54</v>
       </c>
-      <c r="T22">
-        <v>1</v>
-      </c>
       <c r="U22">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V22">
         <v>10</v>
@@ -3758,22 +3821,25 @@
         <v>10</v>
       </c>
       <c r="Y22">
+        <v>10</v>
+      </c>
+      <c r="Z22">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA22">
+      <c r="AB22">
         <v>119</v>
       </c>
-      <c r="AB22">
+      <c r="AC22">
         <v>151</v>
       </c>
-      <c r="AD22">
+      <c r="AE22">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>274</v>
       </c>
@@ -3816,26 +3882,26 @@
       <c r="N23">
         <v>0</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
         <v>104</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>105</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>0.25</v>
       </c>
-      <c r="R23" t="b">
-        <v>0</v>
-      </c>
-      <c r="S23">
+      <c r="S23" t="b">
+        <v>0</v>
+      </c>
+      <c r="T23">
         <v>44</v>
       </c>
-      <c r="T23">
-        <v>1</v>
-      </c>
       <c r="U23">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V23">
         <v>10</v>
@@ -3847,22 +3913,25 @@
         <v>10</v>
       </c>
       <c r="Y23">
+        <v>10</v>
+      </c>
+      <c r="Z23">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z23">
+      <c r="AA23">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA23">
+      <c r="AB23">
         <v>119</v>
       </c>
-      <c r="AB23">
+      <c r="AC23">
         <v>151</v>
       </c>
-      <c r="AD23">
+      <c r="AE23">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>275</v>
       </c>
@@ -3905,26 +3974,26 @@
       <c r="N24">
         <v>0</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24" t="s">
         <v>108</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>109</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>0.05</v>
       </c>
-      <c r="R24" t="b">
-        <v>0</v>
-      </c>
-      <c r="S24">
+      <c r="S24" t="b">
+        <v>0</v>
+      </c>
+      <c r="T24">
         <v>23</v>
       </c>
-      <c r="T24">
-        <v>1</v>
-      </c>
       <c r="U24">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V24">
         <v>10</v>
@@ -3936,22 +4005,25 @@
         <v>10</v>
       </c>
       <c r="Y24">
+        <v>10</v>
+      </c>
+      <c r="Z24">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z24">
+      <c r="AA24">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA24">
+      <c r="AB24">
         <v>119</v>
       </c>
-      <c r="AB24">
+      <c r="AC24">
         <v>151</v>
       </c>
-      <c r="AD24">
+      <c r="AE24">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>276</v>
       </c>
@@ -3994,26 +4066,26 @@
       <c r="N25">
         <v>0</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25" t="s">
         <v>112</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>113</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>0.05</v>
       </c>
-      <c r="R25" t="b">
-        <v>0</v>
-      </c>
-      <c r="S25">
+      <c r="S25" t="b">
+        <v>0</v>
+      </c>
+      <c r="T25">
         <v>7</v>
       </c>
-      <c r="T25">
-        <v>1</v>
-      </c>
       <c r="U25">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V25">
         <v>10</v>
@@ -4025,22 +4097,25 @@
         <v>10</v>
       </c>
       <c r="Y25">
+        <v>10</v>
+      </c>
+      <c r="Z25">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z25">
+      <c r="AA25">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA25">
+      <c r="AB25">
         <v>119</v>
       </c>
-      <c r="AB25">
+      <c r="AC25">
         <v>151</v>
       </c>
-      <c r="AD25">
+      <c r="AE25">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>277</v>
       </c>
@@ -4083,26 +4158,26 @@
       <c r="N26">
         <v>0</v>
       </c>
-      <c r="O26" t="s">
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26" t="s">
         <v>116</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>117</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>0.05</v>
       </c>
-      <c r="R26" t="b">
-        <v>0</v>
-      </c>
-      <c r="S26">
+      <c r="S26" t="b">
+        <v>0</v>
+      </c>
+      <c r="T26">
         <v>29</v>
       </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
       <c r="U26">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V26">
         <v>10</v>
@@ -4114,22 +4189,25 @@
         <v>10</v>
       </c>
       <c r="Y26">
+        <v>10</v>
+      </c>
+      <c r="Z26">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z26">
+      <c r="AA26">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA26">
+      <c r="AB26">
         <v>119</v>
       </c>
-      <c r="AB26">
+      <c r="AC26">
         <v>151</v>
       </c>
-      <c r="AD26">
+      <c r="AE26">
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>278</v>
       </c>
@@ -4172,26 +4250,26 @@
       <c r="N27">
         <v>0</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27" t="s">
         <v>120</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>121</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>0.15</v>
       </c>
-      <c r="R27" t="b">
-        <v>0</v>
-      </c>
-      <c r="S27">
+      <c r="S27" t="b">
+        <v>0</v>
+      </c>
+      <c r="T27">
         <v>46</v>
       </c>
-      <c r="T27">
-        <v>1</v>
-      </c>
       <c r="U27">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V27">
         <v>10</v>
@@ -4203,22 +4281,25 @@
         <v>10</v>
       </c>
       <c r="Y27">
+        <v>10</v>
+      </c>
+      <c r="Z27">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z27">
+      <c r="AA27">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA27">
+      <c r="AB27">
         <v>119</v>
       </c>
-      <c r="AB27">
+      <c r="AC27">
         <v>151</v>
       </c>
-      <c r="AD27">
+      <c r="AE27">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>260</v>
       </c>
@@ -4261,26 +4342,26 @@
       <c r="N28">
         <v>0</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28" t="s">
         <v>124</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>125</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>0.15</v>
       </c>
-      <c r="R28" t="b">
-        <v>0</v>
-      </c>
-      <c r="S28">
+      <c r="S28" t="b">
+        <v>0</v>
+      </c>
+      <c r="T28">
         <v>42</v>
       </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
       <c r="U28">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V28">
         <v>10</v>
@@ -4292,22 +4373,25 @@
         <v>10</v>
       </c>
       <c r="Y28">
+        <v>10</v>
+      </c>
+      <c r="Z28">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z28">
+      <c r="AA28">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA28">
+      <c r="AB28">
         <v>119</v>
       </c>
-      <c r="AB28">
+      <c r="AC28">
         <v>151</v>
       </c>
-      <c r="AD28">
+      <c r="AE28">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>279</v>
       </c>
@@ -4350,26 +4434,26 @@
       <c r="N29">
         <v>0</v>
       </c>
-      <c r="O29" t="s">
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29" t="s">
         <v>128</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>129</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>0.05</v>
       </c>
-      <c r="R29" t="b">
-        <v>0</v>
-      </c>
-      <c r="S29">
+      <c r="S29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T29">
         <v>11</v>
       </c>
-      <c r="T29">
-        <v>1</v>
-      </c>
       <c r="U29">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V29">
         <v>10</v>
@@ -4381,22 +4465,25 @@
         <v>10</v>
       </c>
       <c r="Y29">
+        <v>10</v>
+      </c>
+      <c r="Z29">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z29">
+      <c r="AA29">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA29">
+      <c r="AB29">
         <v>119</v>
       </c>
-      <c r="AB29">
+      <c r="AC29">
         <v>151</v>
       </c>
-      <c r="AD29">
+      <c r="AE29">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>261</v>
       </c>
@@ -4434,31 +4521,31 @@
         <v>125</v>
       </c>
       <c r="M30">
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
       <c r="N30">
         <v>0</v>
       </c>
-      <c r="O30" t="s">
+      <c r="O30">
+        <v>2.7</v>
+      </c>
+      <c r="P30" t="s">
         <v>132</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>133</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>0.05</v>
       </c>
-      <c r="R30" t="b">
-        <v>0</v>
-      </c>
-      <c r="S30">
+      <c r="S30" t="b">
+        <v>0</v>
+      </c>
+      <c r="T30">
         <v>4</v>
       </c>
-      <c r="T30">
-        <v>1</v>
-      </c>
       <c r="U30">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V30">
         <v>10</v>
@@ -4470,22 +4557,25 @@
         <v>10</v>
       </c>
       <c r="Y30">
+        <v>10</v>
+      </c>
+      <c r="Z30">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z30">
+      <c r="AA30">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA30">
+      <c r="AB30">
         <v>119</v>
       </c>
-      <c r="AB30">
+      <c r="AC30">
         <v>151</v>
       </c>
-      <c r="AD30">
+      <c r="AE30">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>262</v>
       </c>
@@ -4528,26 +4618,26 @@
       <c r="N31">
         <v>0</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31" t="s">
         <v>136</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>137</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>0.05</v>
       </c>
-      <c r="R31" t="b">
-        <v>0</v>
-      </c>
-      <c r="S31">
+      <c r="S31" t="b">
+        <v>0</v>
+      </c>
+      <c r="T31">
         <v>9</v>
       </c>
-      <c r="T31">
-        <v>1</v>
-      </c>
       <c r="U31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V31">
         <v>10</v>
@@ -4559,22 +4649,25 @@
         <v>10</v>
       </c>
       <c r="Y31">
+        <v>10</v>
+      </c>
+      <c r="Z31">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z31">
+      <c r="AA31">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA31">
+      <c r="AB31">
         <v>119</v>
       </c>
-      <c r="AB31">
+      <c r="AC31">
         <v>151</v>
       </c>
-      <c r="AD31">
+      <c r="AE31">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>263</v>
       </c>
@@ -4617,26 +4710,26 @@
       <c r="N32">
         <v>0</v>
       </c>
-      <c r="O32" t="s">
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32" t="s">
         <v>140</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>141</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <v>0.05</v>
       </c>
-      <c r="R32" t="b">
-        <v>0</v>
-      </c>
-      <c r="S32">
+      <c r="S32" t="b">
+        <v>0</v>
+      </c>
+      <c r="T32">
         <v>3</v>
       </c>
-      <c r="T32">
-        <v>1</v>
-      </c>
       <c r="U32">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V32">
         <v>10</v>
@@ -4648,22 +4741,25 @@
         <v>10</v>
       </c>
       <c r="Y32">
+        <v>10</v>
+      </c>
+      <c r="Z32">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z32">
+      <c r="AA32">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA32">
+      <c r="AB32">
         <v>119</v>
       </c>
-      <c r="AB32">
+      <c r="AC32">
         <v>151</v>
       </c>
-      <c r="AD32">
+      <c r="AE32">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>280</v>
       </c>
@@ -4706,26 +4802,26 @@
       <c r="N33">
         <v>0</v>
       </c>
-      <c r="O33" t="s">
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33" t="s">
         <v>144</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>145</v>
       </c>
-      <c r="Q33">
-        <v>0</v>
-      </c>
-      <c r="R33" t="b">
-        <v>0</v>
-      </c>
-      <c r="S33">
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33" t="b">
+        <v>0</v>
+      </c>
+      <c r="T33">
         <v>41</v>
       </c>
-      <c r="T33">
-        <v>1</v>
-      </c>
       <c r="U33">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V33">
         <v>10</v>
@@ -4737,22 +4833,25 @@
         <v>10</v>
       </c>
       <c r="Y33">
+        <v>10</v>
+      </c>
+      <c r="Z33">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z33">
+      <c r="AA33">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA33">
+      <c r="AB33">
         <v>119</v>
       </c>
-      <c r="AB33">
+      <c r="AC33">
         <v>151</v>
       </c>
-      <c r="AD33">
+      <c r="AE33">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>281</v>
       </c>
@@ -4795,26 +4894,26 @@
       <c r="N34">
         <v>0</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34" t="s">
         <v>148</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>149</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>0.05</v>
       </c>
-      <c r="R34" t="b">
-        <v>0</v>
-      </c>
-      <c r="S34">
+      <c r="S34" t="b">
+        <v>0</v>
+      </c>
+      <c r="T34">
         <v>8</v>
       </c>
-      <c r="T34">
-        <v>1</v>
-      </c>
       <c r="U34">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V34">
         <v>10</v>
@@ -4826,22 +4925,25 @@
         <v>10</v>
       </c>
       <c r="Y34">
+        <v>10</v>
+      </c>
+      <c r="Z34">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z34">
+      <c r="AA34">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA34">
+      <c r="AB34">
         <v>119</v>
       </c>
-      <c r="AB34">
+      <c r="AC34">
         <v>151</v>
       </c>
-      <c r="AD34">
+      <c r="AE34">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>264</v>
       </c>
@@ -4884,26 +4986,26 @@
       <c r="N35">
         <v>0</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35" t="s">
         <v>152</v>
       </c>
-      <c r="P35" t="s">
+      <c r="Q35" t="s">
         <v>153</v>
       </c>
-      <c r="Q35">
+      <c r="R35">
         <v>0.08</v>
       </c>
-      <c r="R35" t="b">
-        <v>0</v>
-      </c>
-      <c r="S35">
+      <c r="S35" t="b">
+        <v>0</v>
+      </c>
+      <c r="T35">
         <v>48</v>
       </c>
-      <c r="T35">
-        <v>1</v>
-      </c>
       <c r="U35">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V35">
         <v>10</v>
@@ -4915,22 +5017,25 @@
         <v>10</v>
       </c>
       <c r="Y35">
+        <v>10</v>
+      </c>
+      <c r="Z35">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z35">
+      <c r="AA35">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA35">
+      <c r="AB35">
         <v>119</v>
       </c>
-      <c r="AB35">
+      <c r="AC35">
         <v>151</v>
       </c>
-      <c r="AD35">
+      <c r="AE35">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>265</v>
       </c>
@@ -4973,26 +5078,26 @@
       <c r="N36">
         <v>0</v>
       </c>
-      <c r="O36" t="s">
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36" t="s">
         <v>156</v>
       </c>
-      <c r="P36" t="s">
+      <c r="Q36" t="s">
         <v>157</v>
       </c>
-      <c r="Q36">
+      <c r="R36">
         <v>0.05</v>
       </c>
-      <c r="R36" t="b">
-        <v>1</v>
-      </c>
-      <c r="S36">
+      <c r="S36" t="b">
+        <v>1</v>
+      </c>
+      <c r="T36">
         <v>2</v>
       </c>
-      <c r="T36">
-        <v>1</v>
-      </c>
       <c r="U36">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V36">
         <v>10</v>
@@ -5004,22 +5109,25 @@
         <v>10</v>
       </c>
       <c r="Y36">
+        <v>10</v>
+      </c>
+      <c r="Z36">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z36">
+      <c r="AA36">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA36">
+      <c r="AB36">
         <v>119</v>
       </c>
-      <c r="AB36">
+      <c r="AC36">
         <v>151</v>
       </c>
-      <c r="AD36">
+      <c r="AE36">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>266</v>
       </c>
@@ -5062,26 +5170,26 @@
       <c r="N37">
         <v>0</v>
       </c>
-      <c r="O37" t="s">
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37" t="s">
         <v>163</v>
       </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>164</v>
       </c>
-      <c r="Q37">
+      <c r="R37">
         <v>0.05</v>
       </c>
-      <c r="R37" t="b">
-        <v>1</v>
-      </c>
-      <c r="S37">
+      <c r="S37" t="b">
+        <v>1</v>
+      </c>
+      <c r="T37">
         <v>25</v>
       </c>
-      <c r="T37">
-        <v>1</v>
-      </c>
       <c r="U37">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V37">
         <v>10</v>
@@ -5093,18 +5201,21 @@
         <v>10</v>
       </c>
       <c r="Y37">
+        <v>10</v>
+      </c>
+      <c r="Z37">
         <v>0.24149999999999999</v>
       </c>
-      <c r="Z37">
+      <c r="AA37">
         <v>0.15240000000000001</v>
       </c>
-      <c r="AA37">
+      <c r="AB37">
         <v>119</v>
       </c>
-      <c r="AB37">
+      <c r="AC37">
         <v>151</v>
       </c>
-      <c r="AD37">
+      <c r="AE37">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PowerLevelTable 에 equipEfficiency|float! 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A08F77-8B24-4A5B-B9F6-70BD863E1F09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C897EB-60C8-46CA-810C-A45908D808B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
   <sheets>
     <sheet name="ActorTable" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="431">
   <si>
     <t>actorId|String</t>
   </si>
@@ -1312,6 +1312,24 @@
   </si>
   <si>
     <t>checkBurrow|Bool</t>
+  </si>
+  <si>
+    <t>equipEfficiency|float!</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 0.75, 0.65, 0.65, 0.65</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 0.75, 0.7, 0.7, 0.7</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 0.85, 0.8, 0.8, 0.8</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 0.95, 0.9, 0.9, 0.9</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 1, 1, 1</t>
   </si>
 </sst>
 </file>
@@ -1690,7 +1708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAEF85E-644F-4CA8-8208-63C893B0C10A}">
   <dimension ref="A1:AH38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5919,9 +5937,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5005D96F-105D-4071-A89A-95B155F84A28}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5930,7 +5948,7 @@
     <col min="1" max="1" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27" customHeight="1">
+    <row r="1" spans="1:11" ht="27" customHeight="1">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -5961,8 +5979,11 @@
       <c r="J1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5993,8 +6014,11 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6025,8 +6049,11 @@
       <c r="J3">
         <v>300</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6057,8 +6084,11 @@
       <c r="J4">
         <v>800</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6089,8 +6119,11 @@
       <c r="J5">
         <v>1500</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6121,8 +6154,11 @@
       <c r="J6">
         <v>2400</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6153,8 +6189,11 @@
       <c r="J7">
         <v>3500</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6185,8 +6224,11 @@
       <c r="J8">
         <v>4800</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6217,8 +6259,11 @@
       <c r="J9">
         <v>6300</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6249,8 +6294,11 @@
       <c r="J10">
         <v>8000</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6281,8 +6329,11 @@
       <c r="J11">
         <v>10000</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6313,8 +6364,11 @@
       <c r="J12">
         <v>11000</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6345,8 +6399,11 @@
       <c r="J13">
         <v>13000</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6377,8 +6434,11 @@
       <c r="J14">
         <v>14000</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6409,8 +6469,11 @@
       <c r="J15">
         <v>16500</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6441,8 +6504,11 @@
       <c r="J16">
         <v>17500</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6472,6 +6538,9 @@
       </c>
       <c r="J17">
         <v>20000</v>
+      </c>
+      <c r="K17" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HP 미세조정 그릭워리어 0.985 => 1.005 RPG나이트 0.996 => 1.016 걸아처 1.016 => 1.046 에너지실드로봇 0.861 => 0.867
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD54A32-F87D-40FC-836F-72070AFD36F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0699FC90-DA6C-46FF-8DCA-2CF969C66DD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96DE983A-6FA5-4F7F-A108-7CBCD490728B}"/>
   </bookViews>
   <sheets>
     <sheet name="ActorTable" sheetId="1" r:id="rId1"/>
@@ -2914,7 +2914,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0.98499999999999999</v>
+        <v>1.0049999999999999</v>
       </c>
       <c r="I12">
         <v>0.94099999999999995</v>
@@ -4005,7 +4005,7 @@
         <v>1</v>
       </c>
       <c r="H22">
-        <v>0.996</v>
+        <v>1.016</v>
       </c>
       <c r="I22">
         <v>1.054</v>
@@ -4659,7 +4659,7 @@
         <v>2</v>
       </c>
       <c r="H28">
-        <v>1.016</v>
+        <v>1.046</v>
       </c>
       <c r="I28">
         <v>1.171</v>
@@ -4772,7 +4772,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0.86099999999999999</v>
+        <v>0.86699999999999999</v>
       </c>
       <c r="I29">
         <v>0.874</v>

</xml_diff>